<commit_message>
activity feed view status, notifications
</commit_message>
<xml_diff>
--- a/v4/Stored Procedures/noti.xlsx
+++ b/v4/Stored Procedures/noti.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://verdunoilco-my.sharepoint.com/personal/jcodianne_verdunoilco_com/Documents/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\SQL\v4\Stored Procedures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="8_{6737FC74-6107-4166-8669-689609073321}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FFC6ECD2-6633-4E37-A46A-B5271070EAED}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE96D17B-CC12-4F8D-B8B5-064C81B4F975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="40470" yWindow="4350" windowWidth="19005" windowHeight="15345" xr2:uid="{CD823AE6-D738-4E46-9E8B-1971BDE7F262}"/>
+    <workbookView xWindow="3525" yWindow="1110" windowWidth="24780" windowHeight="15975" xr2:uid="{CD823AE6-D738-4E46-9E8B-1971BDE7F262}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
   <si>
     <t>Push</t>
   </si>
@@ -152,10 +152,34 @@
     <t>up_RidePushUserNotification</t>
   </si>
   <si>
-    <t>EXEC up_NotificationRosterEmailDevice 10, 2</t>
-  </si>
-  <si>
-    <t>EXEC up_NotificationRosterEmailDevice 10, 1</t>
+    <t>up_NotificationFriendEmailDevice 1, 1</t>
+  </si>
+  <si>
+    <t>up_NotificationFriendEmailDevice 1, 0</t>
+  </si>
+  <si>
+    <t>up_NotificationRosterEmailDevice 10, 1, 0</t>
+  </si>
+  <si>
+    <t>up_NotificationRosterEmailDevice 10, 2, 0</t>
+  </si>
+  <si>
+    <t>up_NotificationRosterEmailDevice 10, 1, 1</t>
+  </si>
+  <si>
+    <t>up_NotificationRosterEmailDevice 10, 2, 1</t>
+  </si>
+  <si>
+    <t>up_NotificationHubAdminEmailDevice 1, 2</t>
+  </si>
+  <si>
+    <t>up_NotificationHubAdminEmailDevice 1, 1</t>
+  </si>
+  <si>
+    <t>ride invite</t>
+  </si>
+  <si>
+    <t>selection</t>
   </si>
 </sst>
 </file>
@@ -228,9 +252,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -268,7 +292,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -374,7 +398,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -516,7 +540,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -524,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B6DA1F-BD40-4869-AE2B-B15DBDEBDCEC}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -612,10 +636,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -628,6 +652,12 @@
       <c r="C7" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -639,6 +669,12 @@
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -650,6 +686,12 @@
       <c r="C9" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D9" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -661,6 +703,12 @@
       <c r="C10" s="2" t="s">
         <v>26</v>
       </c>
+      <c r="D10" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -672,6 +720,12 @@
       <c r="C11" s="2" t="s">
         <v>27</v>
       </c>
+      <c r="D11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -683,6 +737,12 @@
       <c r="C12" s="2" t="s">
         <v>28</v>
       </c>
+      <c r="D12" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -694,6 +754,12 @@
       <c r="C13" s="2" t="s">
         <v>29</v>
       </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -705,6 +771,12 @@
       <c r="C14" s="2" t="s">
         <v>30</v>
       </c>
+      <c r="D14" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -715,6 +787,23 @@
       </c>
       <c r="C15" s="2" t="s">
         <v>33</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>46</v>
+      </c>
+      <c r="B16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
private checks added on ride lists, user point updates.
private checks added on ride lists, user point updates.
</commit_message>
<xml_diff>
--- a/v4/Stored Procedures/noti.xlsx
+++ b/v4/Stored Procedures/noti.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Documents\GitHub\SQL\v4\Stored Procedures\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE96D17B-CC12-4F8D-B8B5-064C81B4F975}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{160AD499-08CE-4128-AE21-2D8F06545EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3525" yWindow="1110" windowWidth="24780" windowHeight="15975" xr2:uid="{CD823AE6-D738-4E46-9E8B-1971BDE7F262}"/>
+    <workbookView xWindow="3390" yWindow="0" windowWidth="24780" windowHeight="15600" xr2:uid="{CD823AE6-D738-4E46-9E8B-1971BDE7F262}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="50">
   <si>
     <t>Push</t>
   </si>
@@ -149,9 +149,6 @@
     <t>Notifications</t>
   </si>
   <si>
-    <t>up_RidePushUserNotification</t>
-  </si>
-  <si>
     <t>up_NotificationFriendEmailDevice 1, 1</t>
   </si>
   <si>
@@ -180,6 +177,15 @@
   </si>
   <si>
     <t>selection</t>
+  </si>
+  <si>
+    <t>up_RideEmailUserNotification 10</t>
+  </si>
+  <si>
+    <t>up_RidePushUserNotification 10</t>
+  </si>
+  <si>
+    <t>ride like</t>
   </si>
 </sst>
 </file>
@@ -548,7 +554,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85B6DA1F-BD40-4869-AE2B-B15DBDEBDCEC}">
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
@@ -622,7 +628,10 @@
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>37</v>
+        <v>48</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -636,10 +645,10 @@
         <v>24</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -653,10 +662,10 @@
         <v>25</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -670,10 +679,10 @@
         <v>25</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -687,10 +696,10 @@
         <v>26</v>
       </c>
       <c r="D9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -704,10 +713,10 @@
         <v>26</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -721,10 +730,10 @@
         <v>27</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>42</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -738,10 +747,10 @@
         <v>28</v>
       </c>
       <c r="D12" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -755,10 +764,10 @@
         <v>29</v>
       </c>
       <c r="D13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -772,10 +781,10 @@
         <v>30</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -789,21 +798,38 @@
         <v>33</v>
       </c>
       <c r="D15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>38</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
         <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>